<commit_message>
Minor change to template formatting
</commit_message>
<xml_diff>
--- a/ProgramFiles/config_files/1 - CDP Network Audit _ Template.xlsx
+++ b/ProgramFiles/config_files/1 - CDP Network Audit _ Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Pycharm Projects\CDP_Network_Audit-AsyncSSH\ProgramFiles\config_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://muellergroup-my.sharepoint.com/personal/christopher_davies1_muller_co_uk/Documents/Documents/Projects/Python/CDP_Network_Audit/ProgramFiles/config_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2242A986-9D24-4067-AD1B-ED8BAC32EC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2242A986-9D24-4067-AD1B-ED8BAC32EC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A63362D2-7D47-4775-89AE-558BB954DC46}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Audit" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,17 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -852,7 +862,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,8 +897,8 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DNS Resolution Failed">
-      <formula>NOT(ISERROR(SEARCH("DNS Resolution Failed",B1)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="UNRESOLVED">
+      <formula>NOT(ISERROR(SEARCH("UNRESOLVED",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -970,4 +980,10 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{195157b4-6d3a-44f6-8b72-177ae3b6f485}" enabled="1" method="Standard" siteId="{7ea8dd33-ae5f-4280-a7fc-5793d0e74530}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>